<commit_message>
Fix excel date formats
</commit_message>
<xml_diff>
--- a/app/templates/report/reservas.xlsx
+++ b/app/templates/report/reservas.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Data\Development\projects\ciber\cotown\back\app\templates\report\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99D6084A-1219-4836-90C7-AA030919C658}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{25580CCB-A797-41C5-AE25-BABBD7A940C2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="750" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -349,7 +349,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -374,6 +374,9 @@
     <xf numFmtId="4" fontId="2" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="4" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="4" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="2" fillId="6" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="2" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="2" fillId="6" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Hipervínculo 2" xfId="1" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
@@ -774,7 +777,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:BP4"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="13.5" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1116,31 +1121,31 @@
       <c r="E4" s="7"/>
       <c r="F4" s="7"/>
       <c r="G4" s="9"/>
-      <c r="H4" s="10" t="s">
+      <c r="H4" s="16" t="s">
         <v>61</v>
       </c>
-      <c r="I4" s="11" t="s">
+      <c r="I4" s="17" t="s">
         <v>61</v>
       </c>
-      <c r="J4" s="11" t="s">
+      <c r="J4" s="17" t="s">
         <v>61</v>
       </c>
-      <c r="K4" s="11" t="s">
+      <c r="K4" s="17" t="s">
         <v>61</v>
       </c>
-      <c r="L4" s="11" t="s">
+      <c r="L4" s="17" t="s">
         <v>61</v>
       </c>
-      <c r="M4" s="11" t="s">
+      <c r="M4" s="17" t="s">
         <v>61</v>
       </c>
-      <c r="N4" s="11" t="s">
+      <c r="N4" s="17" t="s">
         <v>61</v>
       </c>
-      <c r="O4" s="11" t="s">
+      <c r="O4" s="17" t="s">
         <v>61</v>
       </c>
-      <c r="P4" s="12" t="s">
+      <c r="P4" s="18" t="s">
         <v>61</v>
       </c>
       <c r="Q4" s="13"/>
@@ -1191,7 +1196,7 @@
       <c r="BJ4" s="11"/>
       <c r="BK4" s="11"/>
       <c r="BL4" s="11"/>
-      <c r="BM4" s="11" t="s">
+      <c r="BM4" s="17" t="s">
         <v>61</v>
       </c>
       <c r="BN4" s="11"/>

</xml_diff>